<commit_message>
tdf#161365 xlsx export: checkbox checked property in vmlDrawing.xml
preserve also the checked state while saving

Change-Id: Ibf7e464d952a57c6b52cc74420aa15b24aa0a5d5
Reviewed-on: https://gerrit.libreoffice.org/c/core/+/185872
Reviewed-by: Szymon Kłos <szymon.klos@collabora.com>
Tested-by: Jenkins
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/tdf161365.xlsx
+++ b/sc/qa/unit/data/xlsx/tdf161365.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\checkbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BAC2F31-6F66-4C4B-B8D6-5BEF289048B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9B481A-488C-4B1D-A396-5A829C8160BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07076FF4-2A87-4B04-8FB8-79F97C410235}"/>
   </bookViews>
@@ -50,7 +50,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -60,6 +60,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -77,9 +83,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -100,6 +107,10 @@
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -127,7 +138,74 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78A9B615-98DD-D22F-2172-D5F6B5189A04}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="absolute">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>161925</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>352425</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>285750</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1027" name="Check Box 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1027"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AE76472-41CE-F7D8-6291-457D75355D3A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -471,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21A521C2-C456-45A3-8B09-26241765436F}">
-  <dimension ref="B2:B3"/>
+  <dimension ref="B2:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,13 +560,14 @@
     <col min="2" max="2" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -519,6 +598,28 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1027" r:id="rId4" name="Check Box 4">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="">
+                <anchor>
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>161925</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>85725</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>352425</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>285750</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>

</xml_diff>